<commit_message>
update souces for summary table in sheet "SMART_FY19_Scenario_Common"
</commit_message>
<xml_diff>
--- a/Data/Misc_Scenario_Data_For_CAVESimV10_cases_and_report20191106.xlsx
+++ b/Data/Misc_Scenario_Data_For_CAVESimV10_cases_and_report20191106.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzl/Documents/Papers/2013AutomatedVehicles/2016CAVEnergyModel/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49C4AD94-1731-4A48-9D34-3312AE5316D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F8BBFC-83AB-8C49-A784-D7CB3BE5055E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="900" windowWidth="27020" windowHeight="16540" xr2:uid="{7415CC4D-CF24-9249-8F76-7F24CBAB6216}"/>
+    <workbookView xWindow="2620" yWindow="1380" windowWidth="27020" windowHeight="16540" activeTab="1" xr2:uid="{7415CC4D-CF24-9249-8F76-7F24CBAB6216}"/>
   </bookViews>
   <sheets>
     <sheet name="DemandParams" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="66">
   <si>
     <t>Underserved travelers</t>
   </si>
@@ -161,9 +161,6 @@
     <t>See</t>
   </si>
   <si>
-    <t>SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_VoTT_Factor_Table.xlsx</t>
-  </si>
-  <si>
     <t>Low (.5 - .7)</t>
   </si>
   <si>
@@ -197,20 +194,53 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>='[SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.xlsx]SMART_FY19_Scenario_Common_Assu'!O6</t>
-  </si>
-  <si>
     <t>----------</t>
   </si>
   <si>
     <t>Rough estmations of power requirement vs speed, based only on assumed constant energy use per mile</t>
+  </si>
+  <si>
+    <t>='[SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv]SMART_FY19_Scenario_Common_Assu'!O7</t>
+  </si>
+  <si>
+    <t>='[SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv]SMART_FY19_Scenario_Common_Assu'!O7 -1.0</t>
+  </si>
+  <si>
+    <t>='[SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv]SMART_FY19_Scenario_Common_Assu'!O6</t>
+  </si>
+  <si>
+    <t>='SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_VoTT_Factor_Table.csv'!$E$16</t>
+  </si>
+  <si>
+    <t>`='SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv'!O24</t>
+  </si>
+  <si>
+    <t>`='SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv'!O25</t>
+  </si>
+  <si>
+    <t>`='SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv'!O26</t>
+  </si>
+  <si>
+    <t>`='SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv'!O27</t>
+  </si>
+  <si>
+    <t>`='SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.csv'!O28</t>
+  </si>
+  <si>
+    <t>Needs improvement</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +271,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -273,31 +312,24 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8FFA0B-B673-F643-9342-21DFCEBE403C}">
   <dimension ref="A2:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -699,44 +731,44 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="7" t="s">
-        <v>55</v>
+      <c r="A8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>55</v>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>55</v>
+      <c r="E8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>55</v>
+      <c r="G8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>55</v>
+      <c r="I8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="J8" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>55</v>
+      <c r="K8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="7" t="s">
-        <v>55</v>
+      <c r="M8" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1031,38 +1063,38 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="1" customFormat="1">
-      <c r="A19" s="7" t="s">
-        <v>55</v>
+      <c r="A19" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>55</v>
+      <c r="C19" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>55</v>
+      <c r="E19" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>55</v>
+      <c r="G19" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="H19" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>55</v>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>55</v>
+      <c r="K19" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="1" customFormat="1">
@@ -1290,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BE9BFC-DF11-D443-BCAE-6F5931495360}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1303,202 +1335,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>400</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>400</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>400</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>54</v>
+      <c r="G2" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="4">
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3">
         <v>1900</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1900</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>1900</v>
       </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="4">
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="s">
-        <v>42</v>
+      <c r="G4" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.3</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
         <v>0.3</v>
       </c>
+      <c r="F5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.3</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.6</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="7">
         <v>0.02</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="7">
         <v>0.12</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="7">
         <v>0.12</v>
       </c>
+      <c r="F7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="7">
         <v>1E-3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="7">
         <v>0.115</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7">
         <v>0.115</v>
       </c>
+      <c r="F8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="7">
         <v>1E-3</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="7">
         <v>0.39</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="7">
         <v>0.39</v>
       </c>
+      <c r="F9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
         <v>0.08</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="7">
         <v>0.08</v>
       </c>
+      <c r="F10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
         <v>0.51500000000000001</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="7">
         <v>0.51500000000000001</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1511,14 +1596,19 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>